<commit_message>
Fixed bugs with tunnels
</commit_message>
<xml_diff>
--- a/Tasks list.xlsx
+++ b/Tasks list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1-CITM\Projecta 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elliot\Documents\GitHub\Ms-Pac-Man\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="105">
   <si>
     <t>Name of the task</t>
   </si>
@@ -336,6 +336,9 @@
   </si>
   <si>
     <t>Elliot Jimenez (Gerard)</t>
+  </si>
+  <si>
+    <t>Add-&gt; Time fixing bugs</t>
   </si>
 </sst>
 </file>
@@ -344,14 +347,6 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -397,8 +392,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="22"/>
+      <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -624,32 +626,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -663,18 +662,27 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -693,7 +701,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1081,7 +1088,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$B$62:$B$66</c:f>
+              <c:f>Hoja1!$B$67:$B$71</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1104,7 +1111,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$62:$C$66</c:f>
+              <c:f>Hoja1!$C$67:$C$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1322,7 +1329,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$B$62:$B$66</c:f>
+              <c:f>Hoja1!$B$67:$B$71</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1345,24 +1352,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$D$62:$D$66</c:f>
+              <c:f>Hoja1!$D$67:$D$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>53.400000000000006</c:v>
+                  <c:v>59.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7.1</c:v>
+                  <c:v>13.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1387,7 +1394,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja1!$B$62:$B$66</c:f>
+              <c:f>Hoja1!$B$67:$B$71</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1410,21 +1417,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$E$62:$E$66</c:f>
+              <c:f>Hoja1!$E$67:$E$71</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>87.100000000000009</c:v>
+                  <c:v>111.10000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>41</c:v>
+                  <c:v>74</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.6</c:v>
+                  <c:v>13.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>18</c:v>
@@ -1443,12 +1450,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="140733536"/>
-        <c:axId val="140734096"/>
+        <c:axId val="133341200"/>
+        <c:axId val="133341760"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="140733536"/>
+        <c:axId val="133341200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1485,7 +1492,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140734096"/>
+        <c:crossAx val="133341760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1493,7 +1500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="140734096"/>
+        <c:axId val="133341760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1544,7 +1551,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="140733536"/>
+        <c:crossAx val="133341200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3046,24 +3053,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:I68"/>
+  <dimension ref="A4:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N22" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="43.7109375" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" customWidth="1"/>
     <col min="3" max="3" width="33.28515625" customWidth="1"/>
     <col min="4" max="4" width="29.140625" customWidth="1"/>
     <col min="5" max="5" width="28.28515625" customWidth="1"/>
     <col min="7" max="7" width="31.42578125" customWidth="1"/>
-    <col min="9" max="9" width="32" customWidth="1"/>
+    <col min="9" max="9" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="G4" s="50" t="s">
+      <c r="G4" s="37" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3085,13 +3092,13 @@
       <c r="B7" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D7" s="19">
         <v>1</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="19">
         <v>1</v>
       </c>
     </row>
@@ -3099,13 +3106,13 @@
       <c r="B8" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="20">
         <v>4</v>
       </c>
-      <c r="E8" s="24">
+      <c r="E8" s="21">
         <v>5</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -3119,13 +3126,13 @@
       <c r="B9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="21">
         <v>0.2</v>
       </c>
-      <c r="E9" s="24">
+      <c r="E9" s="21">
         <v>0.2</v>
       </c>
       <c r="G9" s="6" t="s">
@@ -3139,13 +3146,13 @@
       <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="24">
+      <c r="D10" s="21">
         <v>1</v>
       </c>
-      <c r="E10" s="24">
+      <c r="E10" s="21">
         <v>1</v>
       </c>
       <c r="G10" s="7" t="s">
@@ -3159,13 +3166,13 @@
       <c r="B11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="21">
         <v>2</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="21">
         <v>3</v>
       </c>
       <c r="G11" s="7" t="s">
@@ -3179,13 +3186,13 @@
       <c r="B12" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="21">
         <v>0.8</v>
       </c>
-      <c r="E12" s="24">
+      <c r="E12" s="21">
         <v>1</v>
       </c>
       <c r="G12" s="7" t="s">
@@ -3199,13 +3206,13 @@
       <c r="B13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="21">
         <v>0.5</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="21">
         <v>0.5</v>
       </c>
       <c r="G13" s="7" t="s">
@@ -3219,13 +3226,13 @@
       <c r="B14" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="21">
         <v>5</v>
       </c>
-      <c r="E14" s="24">
+      <c r="E14" s="21">
         <v>6</v>
       </c>
       <c r="G14" s="7" t="s">
@@ -3239,13 +3246,13 @@
       <c r="B15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="21">
         <v>4</v>
       </c>
-      <c r="E15" s="24">
+      <c r="E15" s="21">
         <v>4</v>
       </c>
       <c r="G15" s="7" t="s">
@@ -3259,13 +3266,13 @@
       <c r="B16" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="21">
         <v>6</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="21">
         <v>16</v>
       </c>
       <c r="G16" s="7" t="s">
@@ -3279,13 +3286,13 @@
       <c r="B17" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="21">
         <v>2</v>
       </c>
-      <c r="E17" s="24">
+      <c r="E17" s="21">
         <v>2</v>
       </c>
       <c r="G17" s="7" t="s">
@@ -3299,13 +3306,13 @@
       <c r="B18" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="21">
         <v>1</v>
       </c>
-      <c r="E18" s="24">
+      <c r="E18" s="21">
         <v>1</v>
       </c>
       <c r="G18" s="7" t="s">
@@ -3319,13 +3326,13 @@
       <c r="B19" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D19" s="23">
+      <c r="D19" s="20">
         <v>0.1</v>
       </c>
-      <c r="E19" s="24">
+      <c r="E19" s="21">
         <v>0.1</v>
       </c>
       <c r="G19" s="7" t="s">
@@ -3336,13 +3343,13 @@
       <c r="B20" s="12" t="s">
         <v>75</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="23">
+      <c r="D20" s="20">
         <v>0.5</v>
       </c>
-      <c r="E20" s="24">
+      <c r="E20" s="21">
         <v>0.5</v>
       </c>
       <c r="G20" s="7" t="s">
@@ -3353,13 +3360,13 @@
       <c r="B21" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="23">
+      <c r="D21" s="20">
         <v>4</v>
       </c>
-      <c r="E21" s="24">
+      <c r="E21" s="21">
         <v>11</v>
       </c>
       <c r="G21" s="7" t="s">
@@ -3370,13 +3377,13 @@
       <c r="B22" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="23">
+      <c r="D22" s="20">
         <v>0.1</v>
       </c>
-      <c r="E22" s="24">
+      <c r="E22" s="21">
         <v>0.1</v>
       </c>
       <c r="G22" s="7" t="s">
@@ -3387,13 +3394,13 @@
       <c r="B23" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D23" s="23">
+      <c r="D23" s="20">
         <v>2</v>
       </c>
-      <c r="E23" s="24">
+      <c r="E23" s="21">
         <v>3</v>
       </c>
       <c r="G23" s="7" t="s">
@@ -3404,13 +3411,13 @@
       <c r="B24" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="23">
+      <c r="D24" s="20">
         <v>2</v>
       </c>
-      <c r="E24" s="24">
+      <c r="E24" s="21">
         <v>3</v>
       </c>
       <c r="G24" s="7" t="s">
@@ -3421,13 +3428,13 @@
       <c r="B25" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="D25" s="23">
+      <c r="D25" s="20">
         <v>3</v>
       </c>
-      <c r="E25" s="24">
+      <c r="E25" s="21">
         <v>5</v>
       </c>
       <c r="G25" s="7" t="s">
@@ -3438,13 +3445,13 @@
       <c r="B26" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D26" s="23">
+      <c r="D26" s="20">
         <v>0.2</v>
       </c>
-      <c r="E26" s="24">
+      <c r="E26" s="21">
         <v>0.2</v>
       </c>
       <c r="G26" s="7" t="s">
@@ -3452,16 +3459,16 @@
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="23">
+      <c r="D27" s="20">
         <v>0.5</v>
       </c>
-      <c r="E27" s="24">
+      <c r="E27" s="21">
         <v>0.5</v>
       </c>
       <c r="G27" s="7" t="s">
@@ -3469,34 +3476,34 @@
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C28" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="D28" s="33">
-        <v>3</v>
-      </c>
-      <c r="E28" s="33">
-        <v>4</v>
+      <c r="B28" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="20">
+        <v>6</v>
+      </c>
+      <c r="E28" s="21">
+        <v>24</v>
       </c>
       <c r="G28" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C29" s="26" t="s">
+      <c r="B29" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="26">
-        <v>2</v>
-      </c>
-      <c r="E29" s="26">
+      <c r="D29" s="29">
         <v>3</v>
+      </c>
+      <c r="E29" s="29">
+        <v>4</v>
       </c>
       <c r="G29" s="7" t="s">
         <v>24</v>
@@ -3504,517 +3511,588 @@
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D30" s="26">
-        <v>1</v>
-      </c>
-      <c r="E30" s="26">
-        <v>1</v>
+      <c r="D30" s="23">
+        <v>2</v>
+      </c>
+      <c r="E30" s="23">
+        <v>3</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B31" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C31" s="26" t="s">
+      <c r="B31" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D31" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="E31" s="26">
-        <v>0.5</v>
+      <c r="D31" s="23">
+        <v>1</v>
+      </c>
+      <c r="E31" s="23">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D32" s="30">
-        <v>1</v>
-      </c>
-      <c r="E32" s="26">
-        <v>1</v>
+      <c r="D32" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="E32" s="23">
+        <v>0.5</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="C33" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="30">
-        <v>1</v>
-      </c>
-      <c r="E33" s="26">
-        <v>1</v>
+      <c r="D33" s="27">
+        <v>2</v>
+      </c>
+      <c r="E33" s="23">
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="C34" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C34" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D34" s="30">
+      <c r="D34" s="27">
         <v>1</v>
       </c>
-      <c r="E34" s="26">
+      <c r="E34" s="23">
         <v>1</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C35" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="D35" s="30">
-        <v>0.5</v>
-      </c>
-      <c r="E35" s="26">
-        <v>0.5</v>
+        <v>85</v>
+      </c>
+      <c r="C35" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D35" s="27">
+        <v>1</v>
+      </c>
+      <c r="E35" s="23">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="D36" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="E36" s="23">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="C36" s="26" t="s">
+      <c r="C37" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D36" s="30">
+      <c r="D37" s="27">
         <v>1</v>
       </c>
-      <c r="E36" s="26">
+      <c r="E37" s="23">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="15" t="s">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="C37" s="31" t="s">
+      <c r="C38" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="D37" s="32">
-        <v>3</v>
-      </c>
-      <c r="E37" s="31">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C38" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="D38" s="28">
-        <v>1</v>
-      </c>
-      <c r="E38" s="28">
-        <v>1</v>
+      <c r="D38" s="27">
+        <v>8</v>
+      </c>
+      <c r="E38" s="23">
+        <v>20</v>
       </c>
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C39" s="28" t="s">
-        <v>58</v>
+      <c r="B39" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39" s="40" t="s">
+        <v>53</v>
       </c>
       <c r="D39" s="28">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E39" s="28">
-        <v>1</v>
+        <v>24</v>
       </c>
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C40" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="D40" s="28">
-        <v>7</v>
-      </c>
-      <c r="E40" s="28">
-        <v>10</v>
+        <v>57</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40" s="25">
+        <v>1</v>
+      </c>
+      <c r="E40" s="25">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D41" s="25">
+        <v>1</v>
+      </c>
+      <c r="E41" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="25">
+        <v>7</v>
+      </c>
+      <c r="E42" s="25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C41" s="28" t="s">
+      <c r="C43" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D41" s="28">
+      <c r="D43" s="25">
         <v>1</v>
       </c>
-      <c r="E41" s="28">
+      <c r="E43" s="25">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B42" s="12" t="s">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B44" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="C42" s="28" t="s">
+      <c r="C44" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="D42" s="29">
+      <c r="D44" s="26">
         <v>0.5</v>
       </c>
-      <c r="E42" s="28">
+      <c r="E44" s="25">
         <v>0.5</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B43" s="12" t="s">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B45" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C43" s="28" t="s">
+      <c r="C45" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="D43" s="29">
+      <c r="D45" s="26">
         <v>2</v>
       </c>
-      <c r="E43" s="28">
+      <c r="E45" s="25">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="34" t="s">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="D46" s="45">
+        <v>6</v>
+      </c>
+      <c r="E46" s="45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="C44" s="19" t="s">
+      <c r="C47" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D44" s="35">
+      <c r="D47" s="31">
         <v>1</v>
       </c>
-      <c r="E44" s="19">
+      <c r="E47" s="16">
         <v>3</v>
-      </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C45" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D45" s="21">
-        <v>1</v>
-      </c>
-      <c r="E45" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B46" s="12" t="s">
-        <v>76</v>
-      </c>
-      <c r="C46" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D46" s="20">
-        <v>2</v>
-      </c>
-      <c r="E46" s="21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B47" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C47" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D47" s="20">
-        <v>0.5</v>
-      </c>
-      <c r="E47" s="21">
-        <v>0.5</v>
       </c>
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D48" s="18">
+        <v>1</v>
+      </c>
+      <c r="E48" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D49" s="17">
+        <v>2</v>
+      </c>
+      <c r="E49" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B50" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D50" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="E50" s="18">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="C51" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="D48" s="21">
+      <c r="D51" s="18">
         <v>0.1</v>
       </c>
-      <c r="E48" s="21">
+      <c r="E51" s="18">
         <v>0.1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B49" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C49" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D49" s="21">
-        <v>0.5</v>
-      </c>
-      <c r="E49" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C50" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="D50" s="21">
-        <v>2</v>
-      </c>
-      <c r="E50" s="21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="C51" s="36" t="s">
-        <v>51</v>
-      </c>
-      <c r="D51" s="36">
-        <v>1</v>
-      </c>
-      <c r="E51" s="36">
-        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D52" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="E52" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D53" s="18">
+        <v>2</v>
+      </c>
+      <c r="E53" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="15"/>
+      <c r="B54" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D54" s="42">
+        <v>6</v>
+      </c>
+      <c r="E54" s="42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B55" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C55" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="D55" s="32">
+        <v>1</v>
+      </c>
+      <c r="E55" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C52" s="25" t="s">
+      <c r="C56" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="D52" s="25">
+      <c r="D56" s="22">
         <v>1</v>
       </c>
-      <c r="E52" s="25">
+      <c r="E56" s="22">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="12" t="s">
+    <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="C53" s="25" t="s">
+      <c r="C57" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D53" s="27">
+      <c r="D57" s="24">
         <v>1</v>
       </c>
-      <c r="E53" s="25">
+      <c r="E57" s="22">
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="16"/>
-      <c r="B54" s="1" t="s">
+    <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C54" s="25" t="s">
+      <c r="C58" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D54" s="25">
+      <c r="D58" s="22">
         <v>3</v>
       </c>
-      <c r="E54" s="25">
+      <c r="E58" s="22">
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B55" s="2" t="s">
+    <row r="59" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C55" s="37" t="s">
+      <c r="C59" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="D55" s="37">
+      <c r="D59" s="44">
         <v>1</v>
       </c>
-      <c r="E55" s="37">
+      <c r="E59" s="22">
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B56" s="39" t="s">
+    <row r="60" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="C60" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="D60" s="33">
+        <v>6</v>
+      </c>
+      <c r="E60" s="33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="C56" s="17"/>
-      <c r="D56" s="40">
-        <f>SUM(D7:D55)</f>
-        <v>80.5</v>
-      </c>
-      <c r="E56" s="41">
-        <f>SUM(E7:E55)</f>
-        <v>128.19999999999999</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="44" t="s">
+      <c r="C61" s="47"/>
+      <c r="D61" s="48">
+        <f>SUM(D7:D60)</f>
+        <v>116.5</v>
+      </c>
+      <c r="E61" s="49">
+        <f>SUM(E7:E60)</f>
+        <v>191.20000000000002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="50" t="s">
         <v>95</v>
       </c>
-      <c r="C59" s="45"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="46"/>
-    </row>
-    <row r="60" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="47"/>
-      <c r="C60" s="48"/>
-      <c r="D60" s="48"/>
-      <c r="E60" s="49"/>
-    </row>
-    <row r="61" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="38" t="s">
+      <c r="C64" s="51"/>
+      <c r="D64" s="51"/>
+      <c r="E64" s="52"/>
+    </row>
+    <row r="65" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="53"/>
+      <c r="C65" s="54"/>
+      <c r="D65" s="54"/>
+      <c r="E65" s="55"/>
+    </row>
+    <row r="66" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="C61" s="38" t="s">
+      <c r="C66" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="D61" s="38" t="s">
+      <c r="D66" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="E61" s="38" t="s">
+      <c r="E66" s="34" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="34" t="s">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B67" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C62" s="34">
+      <c r="C67" s="30">
         <v>28</v>
       </c>
-      <c r="D62" s="34">
-        <f>(SUM(D40+D42+D47+D49+D53+D54+D55)+SUM(D7:D27))</f>
-        <v>53.400000000000006</v>
-      </c>
-      <c r="E62" s="11">
-        <f>(SUM(E7:E27)+SUM(E40+E42+E47+E49+E53+E54+E55))</f>
-        <v>87.100000000000009</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="12" t="s">
+      <c r="D67" s="30">
+        <f>(SUM(D42+D44+D50+D52+D57+D58+D59)+SUM(D7:D28))</f>
+        <v>59.400000000000006</v>
+      </c>
+      <c r="E67" s="11">
+        <f>(SUM(E7:E28)+SUM(E42+E44+E50+E52+E57+E58+E59))</f>
+        <v>111.10000000000001</v>
+      </c>
+    </row>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B68" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C63" s="12">
+      <c r="C68" s="12">
         <v>10</v>
       </c>
-      <c r="D63" s="12">
-        <f>(SUM(D28:D37)+D16)</f>
-        <v>20</v>
-      </c>
-      <c r="E63" s="1">
-        <f>(SUM(E28:E37)+E16)</f>
-        <v>41</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="12" t="s">
+      <c r="D68" s="12">
+        <f>(SUM(D29:D39)+D16)</f>
+        <v>32</v>
+      </c>
+      <c r="E68" s="1">
+        <f>(SUM(E29:E39)+E16)</f>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B69" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="C64" s="12">
+      <c r="C69" s="12">
         <v>7</v>
       </c>
-      <c r="D64" s="12">
-        <f>(SUM(D38:D43)+D35)</f>
-        <v>13</v>
-      </c>
-      <c r="E64" s="1">
-        <f>(SUM(E38:E43)+E35)</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="65" spans="2:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B65" s="12" t="s">
+      <c r="D69" s="12">
+        <f>(SUM(D40:D46)+D36)</f>
+        <v>19</v>
+      </c>
+      <c r="E69" s="1">
+        <f>(SUM(E40:E46)+E36)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="C65" s="12">
+      <c r="C70" s="12">
         <v>7</v>
       </c>
-      <c r="D65" s="12">
-        <f>SUM(D44:D50)</f>
-        <v>7.1</v>
-      </c>
-      <c r="E65" s="1">
-        <f>SUM(E44:E50)</f>
-        <v>9.6</v>
-      </c>
-    </row>
-    <row r="66" spans="2:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="14" t="s">
+      <c r="D70" s="12">
+        <f>SUM(D47:D54)</f>
+        <v>13.1</v>
+      </c>
+      <c r="E70" s="1">
+        <f>SUM(E47:E54)</f>
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B71" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C66" s="14">
+      <c r="C71" s="14">
         <v>6</v>
       </c>
-      <c r="D66" s="14">
-        <f>(SUM(D51:D55)+D25)</f>
-        <v>10</v>
-      </c>
-      <c r="E66" s="2">
-        <f>(SUM(E51:E55)+E25)</f>
+      <c r="D71" s="14">
+        <f>(SUM(D55:D60)+D25)</f>
+        <v>16</v>
+      </c>
+      <c r="E71" s="2">
+        <f>(SUM(E55:E60)+E25)</f>
         <v>18</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B67" s="13"/>
-    </row>
-    <row r="68" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B68" s="42" t="s">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B72" s="13"/>
+    </row>
+    <row r="73" spans="2:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B73" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="C68" s="42">
+      <c r="C73" s="35">
         <v>58</v>
       </c>
-      <c r="D68" s="3">
-        <f>SUM(D7:D55)</f>
-        <v>80.5</v>
-      </c>
-      <c r="E68" s="43">
-        <f>SUM(E7:E55)</f>
-        <v>128.19999999999999</v>
+      <c r="D73" s="3">
+        <f>SUM(D7:D60)</f>
+        <v>116.5</v>
+      </c>
+      <c r="E73" s="36">
+        <f>SUM(E7:E60)</f>
+        <v>191.20000000000002</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B59:E60"/>
+    <mergeCell ref="B64:E65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed bugs and change directory of sounds and sprites
</commit_message>
<xml_diff>
--- a/Tasks list.xlsx
+++ b/Tasks list.xlsx
@@ -1422,10 +1422,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>99.100000000000009</c:v>
+                  <c:v>97.100000000000009</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65</c:v>
+                  <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19</c:v>
@@ -1450,12 +1450,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="76049808"/>
-        <c:axId val="76049248"/>
+        <c:axId val="89690448"/>
+        <c:axId val="89689888"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="76049808"/>
+        <c:axId val="89690448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1492,7 +1492,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76049248"/>
+        <c:crossAx val="89689888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1500,7 +1500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76049248"/>
+        <c:axId val="89689888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1551,7 +1551,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76049808"/>
+        <c:crossAx val="89690448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3055,8 +3055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3273,7 +3273,7 @@
         <v>6</v>
       </c>
       <c r="E16" s="21">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>11</v>
@@ -3958,7 +3958,7 @@
       </c>
       <c r="E61" s="49">
         <f>SUM(E7:E60)</f>
-        <v>170.20000000000002</v>
+        <v>168.20000000000002</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4004,7 +4004,7 @@
       </c>
       <c r="E67" s="11">
         <f>(SUM(E7:E28)+SUM(E42+E44+E50+E52+E57+E58+E59))</f>
-        <v>99.100000000000009</v>
+        <v>97.100000000000009</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
@@ -4020,7 +4020,7 @@
       </c>
       <c r="E68" s="1">
         <f>(SUM(E29:E39)+E16)</f>
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="69" spans="2:5" x14ac:dyDescent="0.25">
@@ -4087,7 +4087,7 @@
       </c>
       <c r="E73" s="36">
         <f>SUM(E7:E60)</f>
-        <v>170.20000000000002</v>
+        <v>168.20000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bugs in level 4 and change Tasks list
</commit_message>
<xml_diff>
--- a/Tasks list.xlsx
+++ b/Tasks list.xlsx
@@ -1422,19 +1422,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>97.100000000000009</c:v>
+                  <c:v>97.600000000000009</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>63</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>19</c:v>
+                  <c:v>20.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>13.6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1450,12 +1450,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="89690448"/>
-        <c:axId val="89689888"/>
+        <c:axId val="90533424"/>
+        <c:axId val="90532304"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="89690448"/>
+        <c:axId val="90533424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1492,7 +1492,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89689888"/>
+        <c:crossAx val="90532304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1500,7 +1500,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89689888"/>
+        <c:axId val="90532304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1551,7 +1551,7 @@
             <a:endParaRPr lang="es-ES"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89690448"/>
+        <c:crossAx val="90533424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3055,8 +3055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R41" sqref="R41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3663,7 +3663,7 @@
         <v>1</v>
       </c>
       <c r="E40" s="25">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
@@ -3719,7 +3719,7 @@
         <v>0.5</v>
       </c>
       <c r="E44" s="25">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
@@ -3944,7 +3944,7 @@
         <v>6</v>
       </c>
       <c r="E60" s="33">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -3958,7 +3958,7 @@
       </c>
       <c r="E61" s="49">
         <f>SUM(E7:E60)</f>
-        <v>168.20000000000002</v>
+        <v>171.70000000000002</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4004,7 +4004,7 @@
       </c>
       <c r="E67" s="11">
         <f>(SUM(E7:E28)+SUM(E42+E44+E50+E52+E57+E58+E59))</f>
-        <v>97.100000000000009</v>
+        <v>97.600000000000009</v>
       </c>
     </row>
     <row r="68" spans="2:5" x14ac:dyDescent="0.25">
@@ -4036,7 +4036,7 @@
       </c>
       <c r="E69" s="1">
         <f>(SUM(E40:E46)+E36)</f>
-        <v>19</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="70" spans="2:5" x14ac:dyDescent="0.25">
@@ -4068,7 +4068,7 @@
       </c>
       <c r="E71" s="2">
         <f>(SUM(E55:E60)+E25)</f>
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="2:5" x14ac:dyDescent="0.25">
@@ -4087,7 +4087,7 @@
       </c>
       <c r="E73" s="36">
         <f>SUM(E7:E60)</f>
-        <v>168.20000000000002</v>
+        <v>171.70000000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>